<commit_message>
upate with publish package DQbee to PyPI
</commit_message>
<xml_diff>
--- a/Examples/CoupledDuffing/results.xlsx
+++ b/Examples/CoupledDuffing/results.xlsx
@@ -473,10 +473,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.01542782783508301</v>
+        <v>0.01676607131958008</v>
       </c>
       <c r="D2" t="n">
-        <v>0.04726099967956543</v>
+        <v>0.05437588691711426</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -495,10 +495,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>0.06733393669128418</v>
+        <v>0.06878900527954102</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1940176486968994</v>
+        <v>0.2041571140289307</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -517,10 +517,10 @@
         <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>0.204420804977417</v>
+        <v>0.210496187210083</v>
       </c>
       <c r="D4" t="n">
-        <v>0.7248401641845703</v>
+        <v>0.735598087310791</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -539,10 +539,10 @@
         <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4001338481903076</v>
+        <v>0.4108161926269531</v>
       </c>
       <c r="D5" t="n">
-        <v>1.773647308349609</v>
+        <v>1.768811941146851</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -561,10 +561,10 @@
         <v>7</v>
       </c>
       <c r="C6" t="n">
-        <v>0.7203750610351562</v>
+        <v>0.7316422462463379</v>
       </c>
       <c r="D6" t="n">
-        <v>4.452019929885864</v>
+        <v>4.205510854721069</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -580,13 +580,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" t="n">
-        <v>1.101269245147705</v>
+        <v>1.21717095375061</v>
       </c>
       <c r="D7" t="n">
-        <v>10.69215106964111</v>
+        <v>11.14751887321472</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -605,10 +605,10 @@
         <v>10</v>
       </c>
       <c r="C8" t="n">
-        <v>1.777155876159668</v>
+        <v>1.702029943466187</v>
       </c>
       <c r="D8" t="n">
-        <v>29.55974698066711</v>
+        <v>28.27365374565125</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -627,10 +627,10 @@
         <v>12</v>
       </c>
       <c r="C9" t="n">
-        <v>2.514538049697876</v>
+        <v>2.500485897064209</v>
       </c>
       <c r="D9" t="n">
-        <v>80.9920802116394</v>
+        <v>79.25779485702515</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>

</xml_diff>